<commit_message>
This is the commit of completed Personal Task
</commit_message>
<xml_diff>
--- a/Data_Analyst_Batch-53.xlsx
+++ b/Data_Analyst_Batch-53.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohak\Desktop\Yoshops.com\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6615"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="89">
   <si>
     <t>03-07-2023</t>
   </si>
@@ -247,9 +252,6 @@
     <t>Total Effort</t>
   </si>
   <si>
-    <t>SL No.</t>
-  </si>
-  <si>
     <t>Tasks Assignment</t>
   </si>
   <si>
@@ -263,13 +265,34 @@
   </si>
   <si>
     <t>=I11/J11</t>
+  </si>
+  <si>
+    <t>Mohak Singhania</t>
+  </si>
+  <si>
+    <t>Personal Task :-</t>
+  </si>
+  <si>
+    <t>Make Data cleaning in the data and Prepare Bar Graph and Pie Chart Of it.</t>
+  </si>
+  <si>
+    <t>First I install Power BI Desktop and create the file.</t>
+  </si>
+  <si>
+    <t>Personal Task</t>
+  </si>
+  <si>
+    <t>1-50%</t>
+  </si>
+  <si>
+    <t>Complete</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -277,8 +300,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -297,8 +328,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -321,20 +358,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -381,7 +448,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -413,9 +480,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -447,6 +515,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -622,23 +691,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="8" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="7" width="15.7109375" customWidth="1"/>
-    <col min="4" max="73" width="15.7109375" customWidth="1"/>
-    <col min="5" max="72" width="15.7109375" customWidth="1"/>
-    <col min="6" max="7" width="15.7109375" customWidth="1"/>
-    <col min="7" max="32" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="73" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>61</v>
       </c>
@@ -658,7 +725,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:32">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -668,17 +735,34 @@
       <c r="C2" t="s">
         <v>66</v>
       </c>
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>60</v>
+      <c r="D2" s="4">
+        <v>45110</v>
+      </c>
+      <c r="E2" s="4">
+        <v>45170</v>
       </c>
       <c r="H2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:32">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="4">
+        <v>45110</v>
+      </c>
+      <c r="E3" s="4">
+        <v>45170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>69</v>
       </c>
@@ -776,12 +860,26 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:32">
+    <row r="5" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="7" spans="1:32">
+      <c r="B5" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>69</v>
       </c>
@@ -879,12 +977,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:32">
+    <row r="8" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:32" ht="20" customHeight="1">
+    <row r="10" spans="1:32" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G10" s="2" t="s">
         <v>72</v>
       </c>
@@ -901,41 +999,50 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:32">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="G11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H11" t="s">
+        <v>80</v>
+      </c>
+      <c r="I11" t="s">
+        <v>80</v>
+      </c>
+      <c r="J11" t="s">
+        <v>80</v>
+      </c>
+      <c r="K11" t="s">
         <v>81</v>
       </c>
-      <c r="H11" t="s">
-        <v>81</v>
-      </c>
-      <c r="I11" t="s">
-        <v>81</v>
-      </c>
-      <c r="J11" t="s">
-        <v>81</v>
-      </c>
-      <c r="K11" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="12" spans="1:32" ht="20" customHeight="1">
+    </row>
+    <row r="12" spans="1:32" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>63</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:32">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" t="s">
+        <v>88</v>
+      </c>
       <c r="D13" t="s">
         <v>0</v>
       </c>
@@ -943,7 +1050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:32">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>1</v>
       </c>
@@ -951,7 +1058,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:32">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>2</v>
       </c>
@@ -959,7 +1066,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:32">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>3</v>
       </c>
@@ -967,7 +1074,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="4:5">
+    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>4</v>
       </c>
@@ -975,7 +1082,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="4:5">
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
         <v>5</v>
       </c>
@@ -983,7 +1090,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="4:5">
+    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
         <v>6</v>
       </c>
@@ -991,7 +1098,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="4:5">
+    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
         <v>7</v>
       </c>
@@ -999,7 +1106,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="4:5">
+    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>8</v>
       </c>
@@ -1007,7 +1114,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="4:5">
+    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
         <v>9</v>
       </c>
@@ -1015,7 +1122,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="4:5">
+    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>10</v>
       </c>
@@ -1023,7 +1130,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="4:5">
+    <row r="24" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
         <v>11</v>
       </c>
@@ -1031,7 +1138,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="4:5">
+    <row r="25" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
         <v>12</v>
       </c>
@@ -1039,7 +1146,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="4:5">
+    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
         <v>13</v>
       </c>
@@ -1047,7 +1154,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="4:5">
+    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
         <v>14</v>
       </c>
@@ -1055,7 +1162,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="4:5">
+    <row r="28" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
         <v>15</v>
       </c>
@@ -1063,7 +1170,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="4:5">
+    <row r="29" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
         <v>16</v>
       </c>
@@ -1071,7 +1178,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="4:5">
+    <row r="30" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
         <v>17</v>
       </c>
@@ -1079,7 +1186,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="4:5">
+    <row r="31" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
         <v>18</v>
       </c>
@@ -1087,7 +1194,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="4:5">
+    <row r="32" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
         <v>19</v>
       </c>
@@ -1095,7 +1202,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="4:5">
+    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
         <v>20</v>
       </c>
@@ -1103,7 +1210,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="4:5">
+    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
         <v>21</v>
       </c>
@@ -1111,7 +1218,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="4:5">
+    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
         <v>22</v>
       </c>
@@ -1119,7 +1226,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="4:5">
+    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
         <v>23</v>
       </c>
@@ -1127,7 +1234,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="4:5">
+    <row r="37" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
         <v>24</v>
       </c>
@@ -1135,7 +1242,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="4:5">
+    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
         <v>25</v>
       </c>
@@ -1143,7 +1250,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="4:5">
+    <row r="39" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
         <v>26</v>
       </c>
@@ -1151,7 +1258,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="4:5">
+    <row r="40" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
         <v>27</v>
       </c>
@@ -1159,7 +1266,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="4:5">
+    <row r="41" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
         <v>28</v>
       </c>
@@ -1167,7 +1274,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="4:5">
+    <row r="42" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
         <v>29</v>
       </c>
@@ -1175,7 +1282,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="4:5">
+    <row r="43" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
         <v>30</v>
       </c>
@@ -1183,7 +1290,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="44" spans="4:5">
+    <row r="44" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
         <v>31</v>
       </c>
@@ -1191,7 +1298,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="4:5">
+    <row r="45" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
         <v>32</v>
       </c>
@@ -1199,7 +1306,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="46" spans="4:5">
+    <row r="46" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D46" t="s">
         <v>33</v>
       </c>
@@ -1207,7 +1314,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="47" spans="4:5">
+    <row r="47" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
         <v>34</v>
       </c>
@@ -1215,7 +1322,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="4:5">
+    <row r="48" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
         <v>35</v>
       </c>
@@ -1223,7 +1330,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="49" spans="4:5">
+    <row r="49" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
         <v>36</v>
       </c>
@@ -1231,7 +1338,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="4:5">
+    <row r="50" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
         <v>37</v>
       </c>
@@ -1239,7 +1346,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="4:5">
+    <row r="51" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
         <v>38</v>
       </c>
@@ -1247,7 +1354,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="52" spans="4:5">
+    <row r="52" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
         <v>39</v>
       </c>
@@ -1255,7 +1362,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="4:5">
+    <row r="53" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D53" t="s">
         <v>40</v>
       </c>
@@ -1263,7 +1370,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="54" spans="4:5">
+    <row r="54" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
         <v>41</v>
       </c>
@@ -1271,7 +1378,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="55" spans="4:5">
+    <row r="55" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
         <v>42</v>
       </c>
@@ -1279,7 +1386,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="56" spans="4:5">
+    <row r="56" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
         <v>43</v>
       </c>
@@ -1287,7 +1394,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="57" spans="4:5">
+    <row r="57" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D57" t="s">
         <v>44</v>
       </c>
@@ -1295,7 +1402,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="58" spans="4:5">
+    <row r="58" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D58" t="s">
         <v>45</v>
       </c>
@@ -1303,7 +1410,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="59" spans="4:5">
+    <row r="59" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D59" t="s">
         <v>46</v>
       </c>
@@ -1311,7 +1418,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="60" spans="4:5">
+    <row r="60" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
         <v>47</v>
       </c>
@@ -1319,7 +1426,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="61" spans="4:5">
+    <row r="61" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D61" t="s">
         <v>48</v>
       </c>
@@ -1327,7 +1434,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="62" spans="4:5">
+    <row r="62" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D62" t="s">
         <v>49</v>
       </c>
@@ -1335,7 +1442,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="63" spans="4:5">
+    <row r="63" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D63" t="s">
         <v>50</v>
       </c>
@@ -1343,7 +1450,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="64" spans="4:5">
+    <row r="64" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
         <v>51</v>
       </c>
@@ -1351,7 +1458,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="65" spans="4:5">
+    <row r="65" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D65" t="s">
         <v>52</v>
       </c>
@@ -1359,7 +1466,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="66" spans="4:5">
+    <row r="66" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
         <v>53</v>
       </c>
@@ -1367,7 +1474,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="67" spans="4:5">
+    <row r="67" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D67" t="s">
         <v>54</v>
       </c>
@@ -1375,7 +1482,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="68" spans="4:5">
+    <row r="68" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D68" t="s">
         <v>55</v>
       </c>
@@ -1383,7 +1490,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="69" spans="4:5">
+    <row r="69" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D69" t="s">
         <v>56</v>
       </c>
@@ -1391,7 +1498,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="70" spans="4:5">
+    <row r="70" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D70" t="s">
         <v>57</v>
       </c>
@@ -1399,7 +1506,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="71" spans="4:5">
+    <row r="71" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D71" t="s">
         <v>58</v>
       </c>
@@ -1407,7 +1514,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="72" spans="4:5">
+    <row r="72" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D72" t="s">
         <v>59</v>
       </c>
@@ -1415,12 +1522,13 @@
         <v>60</v>
       </c>
     </row>
-    <row r="73" spans="4:5">
+    <row r="73" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D73" t="s">
         <v>60</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>